<commit_message>
Initial commit: Complete project with rebate system and commission features
</commit_message>
<xml_diff>
--- a/维护信息 .xlsx
+++ b/维护信息 .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30720" windowHeight="13380"/>
+    <workbookView windowWidth="30720" windowHeight="13380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="143">
   <si>
     <t>后端代码上传</t>
   </si>
@@ -231,6 +231,9 @@
     <t>苹果玩家下载</t>
   </si>
   <si>
+    <t>后台地址：http://www.tiantian.services</t>
+  </si>
+  <si>
     <t xml:space="preserve"> password: 564bac6d</t>
   </si>
   <si>
@@ -240,24 +243,45 @@
     <t>http://45.207.210.246:55854/fylv1.mobileconfig</t>
   </si>
   <si>
+    <t>商户号：696265672</t>
+  </si>
+  <si>
     <t>系统密码: 7q29t17x31ud</t>
   </si>
   <si>
+    <t>账号：leying</t>
+  </si>
+  <si>
     <t>附加IP: 137.220.153.56</t>
   </si>
   <si>
     <t>安卓玩家下载</t>
   </si>
   <si>
+    <t>密码：a123456</t>
+  </si>
+  <si>
     <t>http://45.207.210.246:55854/fylv1.apk</t>
   </si>
   <si>
+    <t>回调ip  ：47.238.6.73</t>
+  </si>
+  <si>
+    <t>秘钥 ：F63186A18ADBFBF1BD71E906F027B830</t>
+  </si>
+  <si>
+    <t>通道编码：8055</t>
+  </si>
+  <si>
     <t>代理苹果下载</t>
   </si>
   <si>
     <t>http://45.207.210.246:55854/agent1.mobileconfig</t>
   </si>
   <si>
+    <t>网关地址：http://api.tiantian.services/api/v2/gateway</t>
+  </si>
+  <si>
     <t>后端</t>
   </si>
   <si>
@@ -270,25 +294,43 @@
     <t>http://45.207.210.246:55854/agent1.apk</t>
   </si>
   <si>
+    <t>gmall邮箱</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 内网面板地址:     https://110.42.39.85:34816/31852df0</t>
   </si>
   <si>
+    <t>wren33060@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve"> username: fp1u2zae</t>
   </si>
   <si>
+    <t>Bnb159..@</t>
+  </si>
+  <si>
     <t xml:space="preserve"> password: e519fbd9</t>
   </si>
   <si>
+    <t>8006.com</t>
+  </si>
+  <si>
     <t>HB实名认证账号</t>
   </si>
   <si>
     <t>19164034883@163.com</t>
   </si>
   <si>
+    <t>csh88</t>
+  </si>
+  <si>
     <t>洋葱浏览器</t>
   </si>
   <si>
     <t>cEsqh9DLw!,3Bv_</t>
+  </si>
+  <si>
+    <t>Csh199434</t>
   </si>
   <si>
     <t>支付通道</t>
@@ -478,26 +520,18 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Microsoft YaHei"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="11"/>
       <color rgb="FF49B6C3"/>
       <name val="Microsoft YaHei"/>
       <charset val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -513,6 +547,14 @@
       <color rgb="FF000000"/>
       <name val="Microsoft YaHei"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1139,29 +1181,29 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -1563,8 +1605,8 @@
   <sheetPr/>
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10:X18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1586,7 +1628,7 @@
     <col min="31" max="31" width="21.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1" spans="1:29">
+    <row r="1" ht="28" customHeight="1" spans="1:31">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1600,7 +1642,7 @@
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="5"/>
@@ -1612,7 +1654,7 @@
         <v>3</v>
       </c>
       <c r="Q1" s="5"/>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S1" s="5"/>
@@ -1631,7 +1673,7 @@
       <c r="AB1" s="5"/>
       <c r="AC1" s="5"/>
     </row>
-    <row r="2" ht="28" customHeight="1" spans="1:29">
+    <row r="2" ht="28" customHeight="1" spans="1:31">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1662,7 +1704,7 @@
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
     </row>
-    <row r="3" ht="28" customHeight="1" spans="1:29">
+    <row r="3" ht="28" customHeight="1" spans="1:31">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1693,7 +1735,7 @@
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
     </row>
-    <row r="4" ht="17" customHeight="1" spans="1:29">
+    <row r="4" ht="17" customHeight="1" spans="1:31">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1728,7 +1770,7 @@
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
     </row>
-    <row r="5" ht="17" customHeight="1" spans="1:29">
+    <row r="5" ht="17" customHeight="1" spans="1:31">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1759,7 +1801,7 @@
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
     </row>
-    <row r="6" ht="18.35" customHeight="1" spans="1:29">
+    <row r="6" ht="18.35" customHeight="1" spans="1:31">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1787,14 +1829,14 @@
       <c r="Y6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Z6" s="10" t="s">
+      <c r="Z6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
     </row>
-    <row r="7" ht="22.5" customHeight="1" spans="1:29">
+    <row r="7" ht="22.5" customHeight="1" spans="1:31">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1829,7 +1871,7 @@
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
     </row>
-    <row r="8" ht="22.5" customHeight="1" spans="1:29">
+    <row r="8" ht="22.5" customHeight="1" spans="1:31">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1860,7 +1902,7 @@
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
     </row>
-    <row r="9" ht="22.5" customHeight="1" spans="1:29">
+    <row r="9" ht="22.5" customHeight="1" spans="1:31">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1892,704 +1934,704 @@
       <c r="AC9" s="5"/>
     </row>
     <row r="10" ht="22.5" customHeight="1" spans="1:31">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="6" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="11" t="s">
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="6" t="s">
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="11" t="s">
+      <c r="Q10" s="8"/>
+      <c r="R10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12" t="s">
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Z10" s="13">
+      <c r="Z10" s="11">
         <v>13800138009</v>
       </c>
-      <c r="AA10" s="12"/>
-      <c r="AB10" s="12"/>
-      <c r="AC10" s="12"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
       <c r="AE10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" ht="22.5" customHeight="1" spans="1:31">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="12"/>
-      <c r="AC11" s="12"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
       <c r="AE11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" ht="22.5" customHeight="1" spans="1:29">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="12"/>
-      <c r="AA12" s="12"/>
-      <c r="AB12" s="12"/>
-      <c r="AC12" s="12"/>
+    <row r="12" ht="22.5" customHeight="1" spans="1:31">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
     </row>
     <row r="13" ht="11.5" customHeight="1" spans="1:31">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7" t="s">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="12" t="s">
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="12"/>
-      <c r="AC13" s="12"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="10"/>
       <c r="AE13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" ht="11.5" customHeight="1" spans="1:29">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="12"/>
-      <c r="AC14" s="12"/>
+    <row r="14" ht="11.5" customHeight="1" spans="1:31">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
     </row>
     <row r="15" ht="11.5" customHeight="1" spans="1:31">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="Z15" s="12">
+      <c r="Z15" s="10">
         <v>197862</v>
       </c>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="12"/>
-      <c r="AC15" s="12"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
       <c r="AE15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" ht="17" customHeight="1" spans="1:29">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
+    <row r="16" ht="17" customHeight="1" spans="1:31">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="13" t="s">
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="12"/>
-      <c r="AC16" s="12"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
     </row>
     <row r="17" ht="17" customHeight="1" spans="1:29">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="12"/>
-      <c r="AC17" s="12"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
     </row>
     <row r="18" ht="17" customHeight="1" spans="1:29">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="12"/>
-      <c r="Y18" s="12"/>
-      <c r="Z18" s="12"/>
-      <c r="AA18" s="12"/>
-      <c r="AB18" s="12"/>
-      <c r="AC18" s="12"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="10"/>
     </row>
     <row r="19" ht="17" customHeight="1" spans="1:29">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="6" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="11" t="s">
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="6" t="s">
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="11" t="s">
+      <c r="Q19" s="8"/>
+      <c r="R19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="S19" s="12"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="12" t="s">
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Z19" s="13">
+      <c r="Z19" s="11">
         <v>13800000000</v>
       </c>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="12"/>
-      <c r="AC19" s="12"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
     </row>
     <row r="20" ht="17" customHeight="1" spans="1:29">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="12"/>
-      <c r="S20" s="12"/>
-      <c r="T20" s="12"/>
-      <c r="U20" s="12"/>
-      <c r="V20" s="12"/>
-      <c r="W20" s="12"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="12"/>
-      <c r="Z20" s="12"/>
-      <c r="AA20" s="12"/>
-      <c r="AB20" s="12"/>
-      <c r="AC20" s="12"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
     </row>
     <row r="21" ht="17" customHeight="1" spans="1:29">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="12"/>
-      <c r="T21" s="12"/>
-      <c r="U21" s="12"/>
-      <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="12"/>
-      <c r="AA21" s="12"/>
-      <c r="AB21" s="12"/>
-      <c r="AC21" s="12"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
     </row>
     <row r="22" ht="11.5" customHeight="1" spans="1:29">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="12" t="s">
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="12"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
-      <c r="AA22" s="12"/>
-      <c r="AB22" s="12"/>
-      <c r="AC22" s="12"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
     </row>
     <row r="23" ht="11.5" customHeight="1" spans="1:29">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="12"/>
-      <c r="S23" s="12"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
-      <c r="Z23" s="12"/>
-      <c r="AA23" s="12"/>
-      <c r="AB23" s="12"/>
-      <c r="AC23" s="12"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10"/>
     </row>
     <row r="24" ht="11.5" customHeight="1" spans="1:29">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="12"/>
-      <c r="S24" s="12"/>
-      <c r="T24" s="12"/>
-      <c r="U24" s="12"/>
-      <c r="V24" s="12"/>
-      <c r="W24" s="12"/>
-      <c r="X24" s="12"/>
-      <c r="Y24" s="12" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="Z24" s="12">
+      <c r="Z24" s="10">
         <v>123456</v>
       </c>
-      <c r="AA24" s="12"/>
-      <c r="AB24" s="12"/>
-      <c r="AC24" s="12"/>
+      <c r="AA24" s="10"/>
+      <c r="AB24" s="10"/>
+      <c r="AC24" s="10"/>
     </row>
     <row r="25" ht="17" customHeight="1" spans="1:29">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="13" t="s">
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="12"/>
-      <c r="S25" s="12"/>
-      <c r="T25" s="12"/>
-      <c r="U25" s="12"/>
-      <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12"/>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="12"/>
-      <c r="AA25" s="12"/>
-      <c r="AB25" s="12"/>
-      <c r="AC25" s="12"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="10"/>
     </row>
     <row r="26" ht="17" customHeight="1" spans="1:29">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="12"/>
-      <c r="S26" s="12"/>
-      <c r="T26" s="12"/>
-      <c r="U26" s="12"/>
-      <c r="V26" s="12"/>
-      <c r="W26" s="12"/>
-      <c r="X26" s="12"/>
-      <c r="Y26" s="12"/>
-      <c r="Z26" s="12"/>
-      <c r="AA26" s="12"/>
-      <c r="AB26" s="12"/>
-      <c r="AC26" s="12"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="10"/>
     </row>
     <row r="27" ht="17" customHeight="1" spans="1:29">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="12"/>
-      <c r="S27" s="12"/>
-      <c r="T27" s="12"/>
-      <c r="U27" s="12"/>
-      <c r="V27" s="12"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="12"/>
-      <c r="Y27" s="12"/>
-      <c r="Z27" s="12"/>
-      <c r="AA27" s="12"/>
-      <c r="AB27" s="12"/>
-      <c r="AC27" s="12"/>
-    </row>
-    <row r="28" ht="20.4" spans="1:13">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-    </row>
-    <row r="29" ht="20.4" spans="1:13">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-    </row>
-    <row r="30" ht="20.4" spans="1:19">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+    </row>
+    <row r="28" ht="20.4" spans="1:29">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+    </row>
+    <row r="29" ht="20.4" spans="1:29">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+    </row>
+    <row r="30" ht="20.4" spans="1:29">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
       <c r="S30" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" ht="20.4" spans="1:13">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-    </row>
-    <row r="32" ht="20.4" spans="1:19">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
+    <row r="31" ht="20.4" spans="1:29">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+    </row>
+    <row r="32" ht="20.4" spans="1:29">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
       <c r="R32" s="14" t="s">
         <v>25</v>
       </c>
@@ -2598,19 +2640,19 @@
       </c>
     </row>
     <row r="33" ht="20.4" spans="1:19">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
       <c r="R33" s="14" t="s">
         <v>27</v>
       </c>
@@ -2619,36 +2661,36 @@
       </c>
     </row>
     <row r="34" ht="20.4" spans="1:19">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
       <c r="R34" s="14"/>
       <c r="S34" s="14"/>
     </row>
     <row r="35" ht="20.4" spans="1:19">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
       <c r="R35" s="14" t="s">
         <v>29</v>
       </c>
@@ -2657,53 +2699,53 @@
       </c>
     </row>
     <row r="36" ht="20.4" spans="1:19">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
       <c r="R36" s="14"/>
       <c r="S36" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" ht="20.4" spans="1:13">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
+    <row r="37" ht="20.4" spans="1:19">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
     </row>
     <row r="38" ht="20.4" spans="1:19">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
       <c r="R38" s="4" t="s">
         <v>31</v>
       </c>
@@ -2711,7 +2753,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="18:19">
+    <row r="39" spans="1:19">
       <c r="R39" t="s">
         <v>33</v>
       </c>
@@ -2719,7 +2761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="18:19">
+    <row r="40" spans="1:19">
       <c r="R40" t="s">
         <v>8</v>
       </c>
@@ -2799,15 +2841,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S40" sqref="S40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="34.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="60.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="8.66666666666667" customWidth="1"/>
     <col min="3" max="3" width="66.7777777777778" customWidth="1"/>
     <col min="4" max="4" width="41.5555555555556" customWidth="1"/>
@@ -2816,7 +2858,7 @@
     <col min="7" max="7" width="46.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -2830,17 +2872,17 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2851,7 +2893,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2901,7 +2943,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="4:5">
+    <row r="9" spans="1:5">
       <c r="D9" t="s">
         <v>56</v>
       </c>
@@ -2909,7 +2951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="3:4">
+    <row r="11" spans="1:5">
       <c r="C11" t="s">
         <v>58</v>
       </c>
@@ -2917,7 +2959,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="3:4">
+    <row r="12" spans="1:5">
       <c r="C12" t="s">
         <v>59</v>
       </c>
@@ -2925,7 +2967,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="3:4">
+    <row r="13" spans="1:5">
       <c r="C13" t="s">
         <v>61</v>
       </c>
@@ -2933,7 +2975,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="3:5">
+    <row r="14" spans="1:5">
       <c r="C14" t="s">
         <v>63</v>
       </c>
@@ -2944,100 +2986,150 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="3:5">
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="4:4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
       <c r="D16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
       <c r="E18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
       <c r="E21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="E22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="C24" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="C25" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
       <c r="C26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
       <c r="C27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
       <c r="C28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="4:5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
       <c r="C32" s="2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" display="https://137.220.153.55:40090/b4f3d295" tooltip="https://137.220.153.55:40090/b4f3d295"/>
     <hyperlink ref="E7" r:id="rId1" display="https://137.220.153.55:40090/b4f3d295"/>
-    <hyperlink ref="E31" r:id="rId2" display="19164034883@163.com"/>
+    <hyperlink ref="E31" r:id="rId2" display="19164034883@163.com" tooltip="mailto:19164034883@163.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3051,7 +3143,7 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S40" sqref="S40"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -3062,214 +3154,214 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="B11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="B12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="B15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="B16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="B18" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="B22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="B23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="B24" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="B28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="B29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="B30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="B32" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>